<commit_message>
Update Data Center map: add full geocoding support and vivid visualization
- Implemented comprehensive geocoding (Zip code + ArcGIS) to map all 2290 data centers
- Updated interactive map visualization with vivid colors for power plants
- Added latitude/longitude data to datacenters_with_coords.csv
- Cleaned up unused geocoding scripts
</commit_message>
<xml_diff>
--- a/Data Center/KES DC comparison table (1).xlsx
+++ b/Data Center/KES DC comparison table (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m0rim/00_Columbia MBAxMS program/Hackathon/KES-climate-competition/Data Center/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BDAF48-398C-F64E-B45F-5030C0A16452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8977C6B-B2CB-BD47-AD89-88E99DA03976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="660" windowWidth="26760" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2480" yWindow="2080" windowWidth="26760" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="171">
   <si>
     <t>LNG</t>
   </si>
@@ -264,9 +264,6 @@
   </si>
   <si>
     <t>1.10 – 1.12</t>
-  </si>
-  <si>
-    <t>1.25 – 1.40</t>
   </si>
   <si>
     <t>$400M – $500M</t>
@@ -658,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -672,9 +669,6 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1009,7 +1003,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1051,10 +1045,10 @@
         <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>10</v>
@@ -1123,7 +1117,7 @@
         <v>27</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>25</v>
@@ -1132,23 +1126,23 @@
         <v>28</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="O3" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -1159,7 +1153,7 @@
         <v>34</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>31</v>
@@ -1168,7 +1162,7 @@
         <v>32</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>30</v>
@@ -1177,23 +1171,23 @@
         <v>33</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="O4" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -1211,7 +1205,7 @@
         <v>37</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>35</v>
@@ -1220,23 +1214,23 @@
         <v>38</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="O5" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -1244,7 +1238,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="5" t="s">
@@ -1254,7 +1248,7 @@
         <v>42</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>40</v>
@@ -1263,23 +1257,23 @@
         <v>43</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="N6" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="O6" s="12" t="s">
         <v>92</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="O6" s="12" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -1297,7 +1291,7 @@
         <v>46</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>44</v>
@@ -1306,23 +1300,23 @@
         <v>47</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="N7" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="O7" s="12" t="s">
         <v>96</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -1349,14 +1343,14 @@
         <v>52</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>51</v>
@@ -1365,7 +1359,7 @@
         <v>51</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -1383,7 +1377,7 @@
         <v>55</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>53</v>
@@ -1392,11 +1386,11 @@
         <v>56</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>57</v>
@@ -1445,13 +1439,13 @@
         <v>58</v>
       </c>
       <c r="M10" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="O10" s="11" t="s">
         <v>103</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="O10" s="11" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -1469,7 +1463,7 @@
         <v>63</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>61</v>
@@ -1478,31 +1472,31 @@
         <v>64</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N11" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="O11" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="O11" s="11" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>70</v>
+      <c r="B12" s="4">
+        <v>0.88</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="4" t="s">
@@ -1528,36 +1522,36 @@
         <v>69</v>
       </c>
       <c r="L12" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="O12" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>144</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1567,17 +1561,17 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="7"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B14" s="3">
         <v>0.15</v>
@@ -1614,48 +1608,48 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="I15" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="L15" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="M15" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1673,14 +1667,14 @@
       <c r="O16" s="7"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>171</v>
+      <c r="A17" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1694,12 +1688,11 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
-      <c r="C18" s="13"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1715,16 +1708,16 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1732,16 +1725,16 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C21" s="9">
         <v>0.2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="2"/>
@@ -1749,7 +1742,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>57</v>
@@ -1758,7 +1751,7 @@
         <v>0.15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="1"/>
@@ -1766,7 +1759,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>57</v>
@@ -1775,7 +1768,7 @@
         <v>0.2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="2"/>
@@ -1792,7 +1785,7 @@
         <v>0.1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="2"/>
@@ -1800,7 +1793,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>55</v>
@@ -1809,7 +1802,7 @@
         <v>0.1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="2"/>
@@ -1817,16 +1810,16 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C26" s="9">
         <v>0.15</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="2"/>
@@ -1834,16 +1827,16 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C27" s="9">
         <v>0.1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="2"/>

</xml_diff>

<commit_message>
Add FW + Fan cooling simulation mode and update comparison table
</commit_message>
<xml_diff>
--- a/Data Center/KES DC comparison table (1).xlsx
+++ b/Data Center/KES DC comparison table (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m0rim/00_Columbia MBAxMS program/Hackathon/KES-climate-competition/Data Center/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8977C6B-B2CB-BD47-AD89-88E99DA03976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D30746-151B-4843-8622-2EDCDA155E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2480" yWindow="2080" windowWidth="26760" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,9 +56,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="171">
   <si>
-    <t>LNG</t>
-  </si>
-  <si>
     <t>Ship</t>
   </si>
   <si>
@@ -578,6 +575,9 @@
   </si>
   <si>
     <t>ORC + Server coolant</t>
+  </si>
+  <si>
+    <t>LNG (OCR) + CCS</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1003,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1015,543 +1015,543 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="N2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="O3" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="O4" s="11" t="s">
         <v>81</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="O5" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="N6" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="O6" s="12" t="s">
         <v>91</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="O6" s="12" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="I7" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N7" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="O7" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="G8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L8" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O8" s="11" t="s">
         <v>98</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O8" s="11" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="I10" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M10" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="O10" s="11" t="s">
         <v>102</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="O10" s="11" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="N11" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="O11" s="11" t="s">
         <v>107</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="O11" s="11" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4">
         <v>0.88</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="I12" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="O12" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>143</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1561,17 +1561,17 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="7"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B14" s="3">
         <v>0.15</v>
@@ -1608,48 +1608,48 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>133</v>
-      </c>
       <c r="I15" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="L15" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="M15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1668,13 +1668,13 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1688,7 +1688,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -1708,16 +1708,16 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1725,16 +1725,16 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C21" s="9">
         <v>0.2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="2"/>
@@ -1742,16 +1742,16 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="9">
         <v>0.15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="1"/>
@@ -1759,16 +1759,16 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="9">
         <v>0.2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="2"/>
@@ -1776,16 +1776,16 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="9">
         <v>0.1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="2"/>
@@ -1793,16 +1793,16 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="9">
         <v>0.1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="2"/>
@@ -1810,16 +1810,16 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C26" s="9">
         <v>0.15</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="2"/>
@@ -1827,16 +1827,16 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C27" s="9">
         <v>0.1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="2"/>

</xml_diff>